<commit_message>
Array practice questions final change
</commit_message>
<xml_diff>
--- a/testData/ExcelData.xlsx
+++ b/testData/ExcelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samee\Work\Projects\DSAlgo\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB53F061-856B-45A1-A90D-05372F4B3061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FF029F-F72D-48DF-9050-39AA2A232E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2B250AF6-5C6B-4EF8-A5D1-68665084D9EA}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Pythoncode" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>username</t>
   </si>
@@ -80,10 +79,6 @@
     <t>[4, 9, 9, 49, 121]</t>
   </si>
   <si>
-    <t xml:space="preserve">def findMaxConsecutiveOnes(nums) :
- </t>
-  </si>
-  <si>
     <t>def search(input_list, num):
 if(num in input_list):
 print("Element Found")
@@ -96,9 +91,6 @@
   </si>
   <si>
     <t>welcome</t>
-  </si>
-  <si>
-    <t>`</t>
   </si>
   <si>
     <t>Welcome</t>
@@ -217,13 +209,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -584,77 +573,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>26</v>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>26</v>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>26</v>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -670,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B287289B-BD87-4A7D-B4CF-492FB7FD4139}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,10 +703,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -746,7 +735,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
@@ -777,8 +766,8 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
+      <c r="A4" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -809,8 +798,8 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>18</v>
+      <c r="A5" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -841,8 +830,8 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
+      <c r="A6" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -872,9 +861,9 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
+    <row r="7" spans="1:26" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>15</v>
@@ -905,8 +894,8 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>24</v>
+      <c r="A8" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -937,8 +926,8 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>24</v>
+      <c r="A9" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>15</v>
@@ -969,8 +958,8 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>25</v>
+      <c r="A10" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
@@ -1000,9 +989,9 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>15</v>

</xml_diff>